<commit_message>
📝 New sheet for requirements sorted by type and updated use cases
</commit_message>
<xml_diff>
--- a/phases/Requirements/Requirments.xlsx
+++ b/phases/Requirements/Requirments.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laith\University\TM471-A\git repo\Requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Laith\University\TM471-A\git repo\phases\Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D61BA7-20DD-41E5-972C-6E8D2393A9DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE231764-895F-429E-A53C-77FFA49F07DC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FRs" sheetId="1" r:id="rId1"/>
     <sheet name="FRs Cleaning" sheetId="2" r:id="rId2"/>
-    <sheet name="NFRs" sheetId="3" r:id="rId3"/>
+    <sheet name="FRs Cleaning (2)" sheetId="4" r:id="rId3"/>
+    <sheet name="NFRs" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="236">
   <si>
     <t>id</t>
   </si>
@@ -933,6 +934,96 @@
   </si>
   <si>
     <t>FR4</t>
+  </si>
+  <si>
+    <t>FR5</t>
+  </si>
+  <si>
+    <t>FR6</t>
+  </si>
+  <si>
+    <t>FR35</t>
+  </si>
+  <si>
+    <t>FR36</t>
+  </si>
+  <si>
+    <t>FR8</t>
+  </si>
+  <si>
+    <t>FR15</t>
+  </si>
+  <si>
+    <t>FR19</t>
+  </si>
+  <si>
+    <t>FR23</t>
+  </si>
+  <si>
+    <t>FR24</t>
+  </si>
+  <si>
+    <t>FR25</t>
+  </si>
+  <si>
+    <t>FR26</t>
+  </si>
+  <si>
+    <t>FR28</t>
+  </si>
+  <si>
+    <t>FR30</t>
+  </si>
+  <si>
+    <t>FR11</t>
+  </si>
+  <si>
+    <t>FR12</t>
+  </si>
+  <si>
+    <t>FR13</t>
+  </si>
+  <si>
+    <t>FR14</t>
+  </si>
+  <si>
+    <t>FR16</t>
+  </si>
+  <si>
+    <t>FR17</t>
+  </si>
+  <si>
+    <t>FR18</t>
+  </si>
+  <si>
+    <t>FR33</t>
+  </si>
+  <si>
+    <t>FR20</t>
+  </si>
+  <si>
+    <t>FR21</t>
+  </si>
+  <si>
+    <t>FR22</t>
+  </si>
+  <si>
+    <t>FR7</t>
+  </si>
+  <si>
+    <t>FR32</t>
+  </si>
+  <si>
+    <t>FR10</t>
+  </si>
+  <si>
+    <t>FR29</t>
+  </si>
+  <si>
+    <t>FR31</t>
+  </si>
+  <si>
+    <t>FR34</t>
   </si>
 </sst>
 </file>
@@ -1107,7 +1198,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1151,6 +1242,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1165,7 +1259,113 @@
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="15">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -2279,16 +2479,16 @@
       </c>
     </row>
     <row r="50" spans="3:10" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C50" s="15" t="s">
+      <c r="C50" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="D50" s="15"/>
-      <c r="E50" s="15"/>
-      <c r="F50" s="15"/>
-      <c r="G50" s="15"/>
-      <c r="H50" s="15"/>
-      <c r="I50" s="15"/>
-      <c r="J50" s="15"/>
+      <c r="D50" s="16"/>
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="16"/>
+      <c r="H50" s="16"/>
+      <c r="I50" s="16"/>
+      <c r="J50" s="16"/>
     </row>
     <row r="51" spans="3:10" ht="45" x14ac:dyDescent="0.25">
       <c r="C51" s="10" t="s">
@@ -2439,8 +2639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C2D3E01-40A2-497A-AC28-649813C7548F}">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2521,10 +2721,10 @@
       <c r="J2" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="M2" s="16" t="s">
+      <c r="M2" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="N2" s="18" t="s">
         <v>134</v>
       </c>
     </row>
@@ -2556,8 +2756,8 @@
       <c r="J3" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="M3" s="16"/>
-      <c r="N3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="18"/>
     </row>
     <row r="4" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
@@ -3587,6 +3787,1173 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6836DB7-8640-4B86-8372-434800E1BF5D}">
+  <dimension ref="A1:N38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" style="5" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="63.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12" style="15" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" style="15" customWidth="1"/>
+    <col min="8" max="8" width="9" style="15" customWidth="1"/>
+    <col min="9" max="9" width="19.42578125" style="1" customWidth="1"/>
+    <col min="10" max="11" width="11.85546875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="15.7109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="N2" s="18" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="M3" s="17"/>
+      <c r="N3" s="18"/>
+    </row>
+    <row r="4" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="G14" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F20" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F21" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>199</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="G23" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F25" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="G25" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="G26" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="G28" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>197</v>
+      </c>
+      <c r="G30" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="G31" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J31" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="G32" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="G33" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="G34" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J34" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="G35" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J35" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="G36" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J36" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="G37" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J37" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="F38" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G38" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J38" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N2:N3"/>
+  </mergeCells>
+  <conditionalFormatting sqref="J1:J1048576">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+      <formula>"S"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+      <formula>"R"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"O"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="equal">
+      <formula>"A"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+      <formula>"U"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555D7737-055D-47E1-B3C5-9E700893BA8A}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>